<commit_message>
new json csv xlsx
</commit_message>
<xml_diff>
--- a/data/out/cities.xlsx
+++ b/data/out/cities.xlsx
@@ -413,7 +413,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:A6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -421,55 +421,48 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="13" customWidth="1" min="1" max="1"/>
-    <col width="13" customWidth="1" min="2" max="2"/>
+    <col width="30" customWidth="1" min="1" max="1"/>
   </cols>
   <sheetData>
     <row r="1">
       <c r="A1" t="inlineStr">
         <is>
-          <t>Russia</t>
-        </is>
-      </c>
-      <c r="B1" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> USA</t>
+          <t>city country population</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>Moscow</t>
-        </is>
-      </c>
-      <c r="B2" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Calofornia</t>
+          <t>SPB Russia 5384342</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>Ufa</t>
-        </is>
-      </c>
-      <c r="B3" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Florida</t>
+          <t>Moscow Russia 13010112</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>Chelyabinsk</t>
-        </is>
-      </c>
-      <c r="B4" t="inlineStr">
-        <is>
-          <t xml:space="preserve"> Vashington</t>
+          <t>Kazan Russia 1306953</t>
+        </is>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" t="inlineStr">
+        <is>
+          <t>Novosibirsk Russia 1620162</t>
+        </is>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" t="inlineStr">
+        <is>
+          <t>Yekaterinburg Russia 1493749</t>
         </is>
       </c>
     </row>

</xml_diff>